<commit_message>
New train results + updated code
</commit_message>
<xml_diff>
--- a/info-files/statistics/measures_analysis_v2.xlsx
+++ b/info-files/statistics/measures_analysis_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\grodriguez\CardiacOCT\info-files\statistics\second_split\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E00E6CF-9C3C-41C1-808E-30BCB7E8D33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D488B75-F93E-4E51-B707-88D559B89CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plots" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="22">
   <si>
     <t>Model</t>
   </si>
@@ -83,6 +83,27 @@
   </si>
   <si>
     <t>['NLD-AMPH-0017-LAD_frame400', 'NLD-AMPH-0017-LAD_frame458', 'NLD-AMPH-0017-LAD_frame462', 'NLD-AMPH-0017-LAD_frame464', 'NLD-AMPH-0017-LAD_frame469', 'NLD-AMPH-0017-LAD_frame473', 'NLD-AMPH-0017-LAD_frame480', 'NLD-AMPH-0063_frame280', 'NLD-AMPH-0063_frame297', 'NLD-AMPH-0063_frame300', 'NLD-AMPH-0063_frame320', 'NLD-AMPH-0063_frame520']</t>
+  </si>
+  <si>
+    <t>['NLD-AMPH-0017-LAD_frame452', 'NLD-AMPH-0063_frame297', 'NLD-AMPH-0063_frame440', 'NLD-ISALA-0084_frame59', 'NLD-ISALA-0084_frame360', 'NLD-RADB-0024_frame520', 'NLD-RADB-0078_frame40']</t>
+  </si>
+  <si>
+    <t>['NLD-AMPH-0017-LAD_frame462', 'NLD-ISALA-0084_frame360']</t>
+  </si>
+  <si>
+    <t>['NLD-AMPH-0017-LAD_frame462', 'NLD-ISALA-0084_frame360', 'NLD-ISALA-0085_frame120', 'NLD-ISALA-0097_frame360', 'NLD-RADB-0078_frame40']</t>
+  </si>
+  <si>
+    <t>['NLD-AMPH-0017-LAD_frame400', 'NLD-AMPH-0017-LAD_frame458', 'NLD-AMPH-0017-LAD_frame462', 'NLD-AMPH-0017-LAD_frame464', 'NLD-AMPH-0017-LAD_frame469', 'NLD-AMPH-0017-LAD_frame473', 'NLD-AMPH-0017-LAD_frame480', 'NLD-AMPH-0017-LAD_frame520', 'NLD-AMPH-0063_frame280', 'NLD-AMPH-0063_frame290', 'NLD-AMPH-0063_frame297', 'NLD-AMPH-0063_frame300', 'NLD-AMPH-0063_frame520']</t>
+  </si>
+  <si>
+    <t>Pseudo 3D 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>['NLD-AMPH-0017-LAD_frame440', 'NLD-AMPH-0062_frame120', 'NLD-AMPH-0063_frame200', 'NLD-AMPH-0063_frame480', 'NLD-ISALA-0085_frame120', 'NLD-ISALA-0085_frame240', 'NLD-ISALA-0090_frame120', 'NLD-ISALA-0090_frame400', 'NLD-RADB-0063-RCA_frame40', 'NLD-RADB-0063-RCA_frame240', 'NLD-RADB-0063-RCA_frame480', 'NLD-RADB-0078_frame320', 'NLD-RADB-0085_frame80', 'NLD-RADB-0089_frame200']</t>
   </si>
 </sst>
 </file>
@@ -486,23 +507,29 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2</c:f>
+              <c:f>Depth!$A$2:$A$3</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pseudo 3D 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Depth!$G$2</c:f>
+              <c:f>Depth!$G$2:$G$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0.81691548677827541</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9244933865624716</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -546,23 +573,29 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2</c:f>
+              <c:f>Depth!$A$2:$A$3</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pseudo 3D 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Thickness!$G$2</c:f>
+              <c:f>Thickness!$G$2:$G$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0.65008786163045651</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.69586983548136294</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -606,23 +639,29 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2</c:f>
+              <c:f>Depth!$A$2:$A$3</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pseudo 3D 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arc!$G$2</c:f>
+              <c:f>Arc!$G$2:$G$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0.80705995760615212</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83316306134233586</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -944,23 +983,29 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2</c:f>
+              <c:f>Depth!$A$2:$A$3</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pseudo 3D 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Lipid arc'!$G$2</c:f>
+              <c:f>'Lipid arc'!$G$2:$G$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0.73559694968173472</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.72813051932471118</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1004,23 +1049,29 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2</c:f>
+              <c:f>Depth!$A$2:$A$3</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pseudo 3D 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FCT!$G$2</c:f>
+              <c:f>FCT!$G$2:$G$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0.74917523565094302</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.72722837603370283</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1342,23 +1393,29 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2</c:f>
+              <c:f>Depth!$A$2:$A$3</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pseudo 3D 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Depth!$D$2</c:f>
+              <c:f>Depth!$D$2:$D$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>1.0909090909090911</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.577777777777779</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1402,23 +1459,29 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2</c:f>
+              <c:f>Depth!$A$2:$A$3</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pseudo 3D 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Thickness!$D$2</c:f>
+              <c:f>Thickness!$D$2:$D$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>-47.636363636363633</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-42.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1462,23 +1525,29 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2</c:f>
+              <c:f>Depth!$A$2:$A$3</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pseudo 3D 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arc!$D$2</c:f>
+              <c:f>Arc!$D$2:$D$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>-18.11363636363636</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-17.822222222222219</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1800,23 +1869,29 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2</c:f>
+              <c:f>Depth!$A$2:$A$3</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pseudo 3D 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Depth!$E$2</c:f>
+              <c:f>Depth!$E$2:$E$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>68.955788926284356</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45.125252299147633</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1860,23 +1935,29 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2</c:f>
+              <c:f>Depth!$A$2:$A$3</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pseudo 3D 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Thickness!$E$2</c:f>
+              <c:f>Thickness!$E$2:$E$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>209.1265483460684</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>196.03178880534199</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1920,23 +2001,29 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2</c:f>
+              <c:f>Depth!$A$2:$A$3</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pseudo 3D 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arc!$E$2</c:f>
+              <c:f>Arc!$E$2:$E$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>21.974381684434789</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.822305229290262</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2258,23 +2345,29 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2</c:f>
+              <c:f>Depth!$A$2:$A$3</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pseudo 3D 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Lipid arc'!$D$2</c:f>
+              <c:f>'Lipid arc'!$D$2:$D$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>25.36274509803922</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.46078431372549</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2318,23 +2411,29 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2</c:f>
+              <c:f>Depth!$A$2:$A$3</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pseudo 3D 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FCT!$D$2</c:f>
+              <c:f>FCT!$D$2:$D$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>4.833333333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.666666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2656,23 +2755,29 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2</c:f>
+              <c:f>Depth!$A$2:$A$3</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pseudo 3D 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Lipid arc'!$E$2</c:f>
+              <c:f>'Lipid arc'!$E$2:$E$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>55.358154582129522</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.146641705426418</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2716,23 +2821,29 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2</c:f>
+              <c:f>Depth!$A$2:$A$3</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Pseudo 3D 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FCT!$E$2</c:f>
+              <c:f>FCT!$E$2:$E$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>74.426050063835689</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77.213903722740085</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6437,8 +6548,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F7847C3E-E60F-4C77-AF1E-D07C7C554EAC}" name="Table1" displayName="Table1" ref="A1:I2" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A1:I2" xr:uid="{F7847C3E-E60F-4C77-AF1E-D07C7C554EAC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F7847C3E-E60F-4C77-AF1E-D07C7C554EAC}" name="Table1" displayName="Table1" ref="A1:I3" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A1:I3" xr:uid="{F7847C3E-E60F-4C77-AF1E-D07C7C554EAC}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F4C22D2F-D215-4BAA-A39C-212C22D02912}" name="Model"/>
     <tableColumn id="2" xr3:uid="{7005F45F-4D69-49AB-9EC8-769325796BFC}" name="FP"/>
@@ -6455,8 +6566,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1FE82DE7-25CC-48FA-9BB6-E9D39DEC9E30}" name="Table2" displayName="Table2" ref="A1:I2" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
-  <autoFilter ref="A1:I2" xr:uid="{1FE82DE7-25CC-48FA-9BB6-E9D39DEC9E30}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1FE82DE7-25CC-48FA-9BB6-E9D39DEC9E30}" name="Table2" displayName="Table2" ref="A1:I3" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="A1:I3" xr:uid="{1FE82DE7-25CC-48FA-9BB6-E9D39DEC9E30}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{E25EF997-F900-44CD-8A6B-E3739A3327B4}" name="Model"/>
     <tableColumn id="2" xr3:uid="{03BD65A0-29EC-4677-86BB-48231C7EE566}" name="FP"/>
@@ -6473,8 +6584,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{25B3A34A-8511-4EAB-A659-280A416ABD87}" name="Table3" displayName="Table3" ref="A1:I2" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="A1:I2" xr:uid="{25B3A34A-8511-4EAB-A659-280A416ABD87}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{25B3A34A-8511-4EAB-A659-280A416ABD87}" name="Table3" displayName="Table3" ref="A1:I3" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="A1:I3" xr:uid="{25B3A34A-8511-4EAB-A659-280A416ABD87}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B240C185-CCD4-4A15-99D3-716B39673ADB}" name="Model"/>
     <tableColumn id="2" xr3:uid="{FF64CBC7-48F7-47A4-9E3D-4D70827BE4E5}" name="FP"/>
@@ -6491,8 +6602,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F41659BC-FC45-4271-AB3F-2587D8399A01}" name="Table4" displayName="Table4" ref="A1:I2" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A1:I2" xr:uid="{F41659BC-FC45-4271-AB3F-2587D8399A01}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F41659BC-FC45-4271-AB3F-2587D8399A01}" name="Table4" displayName="Table4" ref="A1:I3" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A1:I3" xr:uid="{F41659BC-FC45-4271-AB3F-2587D8399A01}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{11CA475A-8834-46D1-B193-71A66A26AFC0}" name="Model"/>
     <tableColumn id="2" xr3:uid="{0997532C-545B-4163-812E-33BE03D153B5}" name="FP"/>
@@ -6509,8 +6620,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6CF91DCA-A2A6-43F5-AAB1-94F7DA965C3C}" name="Table5" displayName="Table5" ref="A1:I2" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:I2" xr:uid="{6CF91DCA-A2A6-43F5-AAB1-94F7DA965C3C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6CF91DCA-A2A6-43F5-AAB1-94F7DA965C3C}" name="Table5" displayName="Table5" ref="A1:I3" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:I3" xr:uid="{6CF91DCA-A2A6-43F5-AAB1-94F7DA965C3C}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BDF23567-2CC8-4F6C-A5E1-4780C5C307B8}" name="Model"/>
     <tableColumn id="2" xr3:uid="{64FAC5C0-B97C-490C-B0E9-9FD5F6EE4BD0}" name="FP"/>
@@ -6811,14 +6922,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6637BE2-E0E7-4739-BE8A-ECD39922EFEF}">
-  <dimension ref="A1"/>
+  <dimension ref="T42"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="T42" sqref="T42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="42" spans="20:20" x14ac:dyDescent="0.3">
+      <c r="T42" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -6826,10 +6943,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6903,6 +7020,35 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>15.577777777777779</v>
+      </c>
+      <c r="E3">
+        <v>45.125252299147633</v>
+      </c>
+      <c r="F3">
+        <v>0.93810568769754166</v>
+      </c>
+      <c r="G3">
+        <v>0.9244933865624716</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
@@ -6913,10 +7059,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6990,6 +7136,35 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>-17.822222222222219</v>
+      </c>
+      <c r="E3">
+        <v>20.822305229290262</v>
+      </c>
+      <c r="F3">
+        <v>0.90495243673776982</v>
+      </c>
+      <c r="G3">
+        <v>0.83316306134233586</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
@@ -7000,10 +7175,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7077,6 +7252,35 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>-42.6</v>
+      </c>
+      <c r="E3">
+        <v>196.03178880534199</v>
+      </c>
+      <c r="F3">
+        <v>0.70092672477234075</v>
+      </c>
+      <c r="G3">
+        <v>0.69586983548136294</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
@@ -7087,10 +7291,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7164,6 +7368,35 @@
         <v>13</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>2.666666666666667</v>
+      </c>
+      <c r="E3">
+        <v>77.213903722740085</v>
+      </c>
+      <c r="F3">
+        <v>0.72726345512183421</v>
+      </c>
+      <c r="G3">
+        <v>0.72722837603370283</v>
+      </c>
+      <c r="H3">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
@@ -7174,10 +7407,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7251,6 +7484,35 @@
         <v>14</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>25.46078431372549</v>
+      </c>
+      <c r="E3">
+        <v>57.146641705426418</v>
+      </c>
+      <c r="F3">
+        <v>0.78004554169218332</v>
+      </c>
+      <c r="G3">
+        <v>0.72813051932471118</v>
+      </c>
+      <c r="H3">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Update scripts + readme + info files
</commit_message>
<xml_diff>
--- a/info-files/statistics/measures_analysis_v2.xlsx
+++ b/info-files/statistics/measures_analysis_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\grodriguez\CardiacOCT\info-files\statistics\second_split\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D488B75-F93E-4E51-B707-88D559B89CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DE26A0-3B04-446B-89B0-8553BC86A6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plots" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="28">
   <si>
     <t>Model</t>
   </si>
@@ -105,12 +105,30 @@
   <si>
     <t>['NLD-AMPH-0017-LAD_frame440', 'NLD-AMPH-0062_frame120', 'NLD-AMPH-0063_frame200', 'NLD-AMPH-0063_frame480', 'NLD-ISALA-0085_frame120', 'NLD-ISALA-0085_frame240', 'NLD-ISALA-0090_frame120', 'NLD-ISALA-0090_frame400', 'NLD-RADB-0063-RCA_frame40', 'NLD-RADB-0063-RCA_frame240', 'NLD-RADB-0063-RCA_frame480', 'NLD-RADB-0078_frame320', 'NLD-RADB-0085_frame80', 'NLD-RADB-0089_frame200']</t>
   </si>
+  <si>
+    <t>Pseudo 3D 2</t>
+  </si>
+  <si>
+    <t>['NLD-AMPH-0017-LAD_frame452', 'NLD-AMPH-0063_frame297', 'NLD-AMPH-0063_frame440', 'NLD-ISALA-0084_frame59', 'NLD-ISALA-0084_frame360', 'NLD-RADB-0024_frame320', 'NLD-RADB-0024_frame520', 'NLD-RADB-0078_frame280']</t>
+  </si>
+  <si>
+    <t>['NLD-AMPH-0017-LAD_frame462']</t>
+  </si>
+  <si>
+    <t>['NLD-AMPH-0017-LAD_frame462', 'NLD-ISALA-0084_frame360', 'NLD-ISALA-0085_frame120', 'NLD-ISALA-0097_frame360', 'NLD-RADB-0078_frame280']</t>
+  </si>
+  <si>
+    <t>['NLD-AMPH-0062_frame120', 'NLD-AMPH-0063_frame200', 'NLD-ISALA-0090_frame0', 'NLD-ISALA-0090_frame400', 'NLD-RADB-0063-RCA_frame40', 'NLD-RADB-0078_frame320', 'NLD-RADB-0089_frame200']</t>
+  </si>
+  <si>
+    <t>['NLD-AMPH-0017-LAD_frame400', 'NLD-AMPH-0017-LAD_frame458', 'NLD-AMPH-0017-LAD_frame462', 'NLD-AMPH-0017-LAD_frame464', 'NLD-AMPH-0017-LAD_frame469', 'NLD-AMPH-0017-LAD_frame473', 'NLD-AMPH-0017-LAD_frame475', 'NLD-AMPH-0017-LAD_frame480', 'NLD-AMPH-0017-LAD_frame520', 'NLD-AMPH-0063_frame280', 'NLD-AMPH-0063_frame290', 'NLD-AMPH-0063_frame297', 'NLD-AMPH-0063_frame300', 'NLD-AMPH-0063_frame320', 'NLD-AMPH-0063_frame520', 'NLD-AMPH-0063_frame522', 'NLD-RADB-0078_frame320']</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +149,12 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -507,29 +531,35 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2:$A$3</c:f>
+              <c:f>Depth!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Pseudo 3D 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pseudo 3D 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Depth!$G$2:$G$3</c:f>
+              <c:f>Depth!$G$2:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.81691548677827541</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.9244933865624716</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7348843373594699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -573,29 +603,35 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2:$A$3</c:f>
+              <c:f>Depth!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Pseudo 3D 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pseudo 3D 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Thickness!$G$2:$G$3</c:f>
+              <c:f>Thickness!$G$2:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.65008786163045651</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.69586983548136294</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.63129811765639277</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -639,29 +675,35 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2:$A$3</c:f>
+              <c:f>Depth!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Pseudo 3D 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pseudo 3D 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arc!$G$2:$G$3</c:f>
+              <c:f>Arc!$G$2:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.80705995760615212</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.83316306134233586</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.79776360879524366</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -983,29 +1025,35 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2:$A$3</c:f>
+              <c:f>Depth!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Pseudo 3D 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pseudo 3D 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Lipid arc'!$G$2:$G$3</c:f>
+              <c:f>'Lipid arc'!$G$2:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.73559694968173472</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.72813051932471118</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.74524406883309013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1049,29 +1097,35 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2:$A$3</c:f>
+              <c:f>Depth!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Pseudo 3D 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pseudo 3D 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FCT!$G$2:$G$3</c:f>
+              <c:f>FCT!$G$2:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.74917523565094302</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.72722837603370283</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75666584509166945</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1393,29 +1447,35 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2:$A$3</c:f>
+              <c:f>Depth!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Pseudo 3D 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pseudo 3D 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Depth!$D$2:$D$3</c:f>
+              <c:f>Depth!$D$2:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1.0909090909090911</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>15.577777777777779</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29.212765957446809</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1459,29 +1519,35 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2:$A$3</c:f>
+              <c:f>Depth!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Pseudo 3D 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pseudo 3D 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Thickness!$D$2:$D$3</c:f>
+              <c:f>Thickness!$D$2:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>-47.636363636363633</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-42.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-50.936170212765958</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1525,29 +1591,35 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2:$A$3</c:f>
+              <c:f>Depth!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Pseudo 3D 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pseudo 3D 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arc!$D$2:$D$3</c:f>
+              <c:f>Arc!$D$2:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>-18.11363636363636</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-17.822222222222219</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-19.191489361702128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1869,29 +1941,35 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2:$A$3</c:f>
+              <c:f>Depth!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Pseudo 3D 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pseudo 3D 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Depth!$E$2:$E$3</c:f>
+              <c:f>Depth!$E$2:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>68.955788926284356</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>45.125252299147633</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>91.424177669598151</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1935,29 +2013,35 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2:$A$3</c:f>
+              <c:f>Depth!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Pseudo 3D 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pseudo 3D 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Thickness!$E$2:$E$3</c:f>
+              <c:f>Thickness!$E$2:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>209.1265483460684</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>196.03178880534199</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>223.96631626067179</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2001,29 +2085,35 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2:$A$3</c:f>
+              <c:f>Depth!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Pseudo 3D 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pseudo 3D 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Arc!$E$2:$E$3</c:f>
+              <c:f>Arc!$E$2:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>21.974381684434789</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>20.822305229290262</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.820892161753829</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2345,29 +2435,35 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2:$A$3</c:f>
+              <c:f>Depth!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Pseudo 3D 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pseudo 3D 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Lipid arc'!$D$2:$D$3</c:f>
+              <c:f>'Lipid arc'!$D$2:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>25.36274509803922</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>25.46078431372549</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.1078431372549</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2411,29 +2507,35 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2:$A$3</c:f>
+              <c:f>Depth!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Pseudo 3D 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pseudo 3D 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FCT!$D$2:$D$3</c:f>
+              <c:f>FCT!$D$2:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>4.833333333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.97058823529411764</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2755,29 +2857,35 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2:$A$3</c:f>
+              <c:f>Depth!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Pseudo 3D 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pseudo 3D 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Lipid arc'!$E$2:$E$3</c:f>
+              <c:f>'Lipid arc'!$E$2:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>55.358154582129522</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>57.146641705426418</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>54.552170903181327</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2821,29 +2929,35 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Depth!$A$2:$A$3</c:f>
+              <c:f>Depth!$A$2:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>RGB 2D</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Pseudo 3D 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Pseudo 3D 2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>FCT!$E$2:$E$3</c:f>
+              <c:f>FCT!$E$2:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>74.426050063835689</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>77.213903722740085</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71.731177879957727</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6548,8 +6662,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F7847C3E-E60F-4C77-AF1E-D07C7C554EAC}" name="Table1" displayName="Table1" ref="A1:I3" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
-  <autoFilter ref="A1:I3" xr:uid="{F7847C3E-E60F-4C77-AF1E-D07C7C554EAC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F7847C3E-E60F-4C77-AF1E-D07C7C554EAC}" name="Table1" displayName="Table1" ref="A1:I4" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
+  <autoFilter ref="A1:I4" xr:uid="{F7847C3E-E60F-4C77-AF1E-D07C7C554EAC}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{F4C22D2F-D215-4BAA-A39C-212C22D02912}" name="Model"/>
     <tableColumn id="2" xr3:uid="{7005F45F-4D69-49AB-9EC8-769325796BFC}" name="FP"/>
@@ -6566,8 +6680,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1FE82DE7-25CC-48FA-9BB6-E9D39DEC9E30}" name="Table2" displayName="Table2" ref="A1:I3" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
-  <autoFilter ref="A1:I3" xr:uid="{1FE82DE7-25CC-48FA-9BB6-E9D39DEC9E30}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1FE82DE7-25CC-48FA-9BB6-E9D39DEC9E30}" name="Table2" displayName="Table2" ref="A1:I4" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="A1:I4" xr:uid="{1FE82DE7-25CC-48FA-9BB6-E9D39DEC9E30}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{E25EF997-F900-44CD-8A6B-E3739A3327B4}" name="Model"/>
     <tableColumn id="2" xr3:uid="{03BD65A0-29EC-4677-86BB-48231C7EE566}" name="FP"/>
@@ -6584,8 +6698,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{25B3A34A-8511-4EAB-A659-280A416ABD87}" name="Table3" displayName="Table3" ref="A1:I3" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="A1:I3" xr:uid="{25B3A34A-8511-4EAB-A659-280A416ABD87}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{25B3A34A-8511-4EAB-A659-280A416ABD87}" name="Table3" displayName="Table3" ref="A1:I4" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="A1:I4" xr:uid="{25B3A34A-8511-4EAB-A659-280A416ABD87}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B240C185-CCD4-4A15-99D3-716B39673ADB}" name="Model"/>
     <tableColumn id="2" xr3:uid="{FF64CBC7-48F7-47A4-9E3D-4D70827BE4E5}" name="FP"/>
@@ -6602,8 +6716,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F41659BC-FC45-4271-AB3F-2587D8399A01}" name="Table4" displayName="Table4" ref="A1:I3" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A1:I3" xr:uid="{F41659BC-FC45-4271-AB3F-2587D8399A01}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F41659BC-FC45-4271-AB3F-2587D8399A01}" name="Table4" displayName="Table4" ref="A1:I4" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A1:I4" xr:uid="{F41659BC-FC45-4271-AB3F-2587D8399A01}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{11CA475A-8834-46D1-B193-71A66A26AFC0}" name="Model"/>
     <tableColumn id="2" xr3:uid="{0997532C-545B-4163-812E-33BE03D153B5}" name="FP"/>
@@ -6620,8 +6734,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6CF91DCA-A2A6-43F5-AAB1-94F7DA965C3C}" name="Table5" displayName="Table5" ref="A1:I3" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:I3" xr:uid="{6CF91DCA-A2A6-43F5-AAB1-94F7DA965C3C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{6CF91DCA-A2A6-43F5-AAB1-94F7DA965C3C}" name="Table5" displayName="Table5" ref="A1:I4" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:I4" xr:uid="{6CF91DCA-A2A6-43F5-AAB1-94F7DA965C3C}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{BDF23567-2CC8-4F6C-A5E1-4780C5C307B8}" name="Model"/>
     <tableColumn id="2" xr3:uid="{64FAC5C0-B97C-490C-B0E9-9FD5F6EE4BD0}" name="FP"/>
@@ -6924,8 +7038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6637BE2-E0E7-4739-BE8A-ECD39922EFEF}">
   <dimension ref="T42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="T42" sqref="T42"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6943,10 +7057,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7049,6 +7163,35 @@
         <v>15</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>29.212765957446809</v>
+      </c>
+      <c r="E4">
+        <v>91.424177669598151</v>
+      </c>
+      <c r="F4">
+        <v>0.77645902037665526</v>
+      </c>
+      <c r="G4">
+        <v>0.7348843373594699</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
@@ -7059,10 +7202,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7165,6 +7308,35 @@
         <v>16</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>-19.191489361702128</v>
+      </c>
+      <c r="E4">
+        <v>22.820892161753829</v>
+      </c>
+      <c r="F4">
+        <v>0.88054023204321963</v>
+      </c>
+      <c r="G4">
+        <v>0.79776360879524366</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
@@ -7175,10 +7347,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7281,6 +7453,35 @@
         <v>17</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>-50.936170212765958</v>
+      </c>
+      <c r="E4">
+        <v>223.96631626067179</v>
+      </c>
+      <c r="F4">
+        <v>0.64046782044074557</v>
+      </c>
+      <c r="G4">
+        <v>0.63129811765639277</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
@@ -7291,10 +7492,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7397,6 +7598,35 @@
         <v>21</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>-0.97058823529411764</v>
+      </c>
+      <c r="E4">
+        <v>71.731177879957727</v>
+      </c>
+      <c r="F4">
+        <v>0.75920568404815025</v>
+      </c>
+      <c r="G4">
+        <v>0.75666584509166945</v>
+      </c>
+      <c r="H4">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
@@ -7407,10 +7637,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7513,7 +7743,37 @@
         <v>18</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>25.1078431372549</v>
+      </c>
+      <c r="E4">
+        <v>54.552170903181327</v>
+      </c>
+      <c r="F4">
+        <v>0.79577604500166299</v>
+      </c>
+      <c r="G4">
+        <v>0.74524406883309013</v>
+      </c>
+      <c r="H4">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>